<commit_message>
Basic Kalibration for voltage
</commit_message>
<xml_diff>
--- a/otherinfos/Kalibration/DruckSensor.xlsx
+++ b/otherinfos/Kalibration/DruckSensor.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74BB26F-9FEC-42E1-A2A3-0E1CD3EE6F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0EF533F-498A-42C8-A1CE-5EE8E7F824F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>Gewicht [kg]</t>
   </si>
@@ -85,9 +85,6 @@
     <t>Aufsteigende Mittelwerte [mV]</t>
   </si>
   <si>
-    <t>Wasserhöhe [m]</t>
-  </si>
-  <si>
     <t>1m = 0,1bar = 9,80665</t>
   </si>
   <si>
@@ -103,7 +100,31 @@
     <t>Kontrolle via PSI / kpa</t>
   </si>
   <si>
-    <t>Empfindlichkeit [(mV/V)/PSI]</t>
+    <t>Druck [mmHg]</t>
+  </si>
+  <si>
+    <t>Empfindlichkeit [(mV/V)/mmHg]</t>
+  </si>
+  <si>
+    <t>1mmHg = 133,322 Pa</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>mmHg</t>
+  </si>
+  <si>
+    <t>Multimeter</t>
+  </si>
+  <si>
+    <t>Arduino</t>
+  </si>
+  <si>
+    <t>Max bei 299,947mmHg</t>
+  </si>
+  <si>
+    <t>1mmHg=1/51,715 PSI</t>
   </si>
 </sst>
 </file>
@@ -139,7 +160,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -288,19 +309,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -387,12 +395,83 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -401,9 +480,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -419,40 +495,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
@@ -467,30 +546,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -648,34 +725,61 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Sensor 1'!$B$4:$B$14</c:f>
+              <c:f>'Sensor 1'!$B$4:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>295</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Sensor 1'!$F$4:$F$14</c:f>
+              <c:f>'Sensor 1'!$F$4:$F$17</c:f>
               <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:formatCode>00,000</c:formatCode>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -707,6 +811,15 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -769,20 +882,82 @@
             <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
-            <c:numRef>
+            <c:strRef>
               <c:f>'Sensor 1'!$B$19:$B$29</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="11"/>
-              </c:numCache>
-            </c:numRef>
+                <c:pt idx="0">
+                  <c:v>Absteigend</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Druck [mmHg]</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>'Sensor 1'!$F$19:$F$29</c:f>
               <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
+                <c:formatCode>00,000</c:formatCode>
                 <c:ptCount val="11"/>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -997,7 +1172,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:numFmt formatCode="00,000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1258,16 +1433,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>250</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1371,20 +1564,82 @@
             <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
-            <c:numRef>
+            <c:strRef>
               <c:f>'Sensor 1'!$B$19:$B$29</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="11"/>
-              </c:numCache>
-            </c:numRef>
+                <c:pt idx="0">
+                  <c:v>Absteigend</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Druck [mmHg]</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>'Sensor 1'!$H$19:$H$29</c:f>
               <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.0000">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.0000">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.0000">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.0000">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.0000">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.0000">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.0000">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.0000">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.0000">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1860,16 +2115,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>250</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1973,20 +2246,82 @@
             <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
-            <c:numRef>
+            <c:strRef>
               <c:f>'Sensor 1'!$B$19:$B$29</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="11"/>
-              </c:numCache>
-            </c:numRef>
+                <c:pt idx="0">
+                  <c:v>Absteigend</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Druck [mmHg]</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
               <c:f>'Sensor 1'!$I$19:$I$29</c:f>
               <c:numCache>
-                <c:formatCode>0.0000%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.0000%">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.0000%">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.0000%">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.0000%">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.0000%">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.0000%">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.0000%">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.0000%">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.0000%">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -7754,16 +8089,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>613799</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>9270</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>40968</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>29754</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>18333</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>141954</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>602123</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>172681</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8245,28 +8580,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:M34"/>
+  <dimension ref="B1:W34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="29" t="s">
         <v>1</v>
       </c>
@@ -8277,586 +8615,960 @@
       <c r="G2" s="30"/>
       <c r="H2" s="30"/>
       <c r="I2" s="31"/>
-      <c r="J2" t="s">
-        <v>18</v>
+      <c r="K2" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="41"/>
+      <c r="M2" s="42"/>
+      <c r="O2" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="27" t="s">
+    <row r="3" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="28" t="s">
+      <c r="I3" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="M3" s="41" t="s">
-        <v>22</v>
+      <c r="K3" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="45" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="20">
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B4" s="18">
         <v>0</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="22">
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="20">
         <f>(C4+D4+E4)/3</f>
         <v>0</v>
       </c>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22">
+      <c r="G4" s="20"/>
+      <c r="H4" s="20">
         <f>MAX(C4-F4,D4-F4,E4-F4)*1000</f>
         <v>0</v>
       </c>
-      <c r="I4" s="23" t="e">
+      <c r="I4" s="21" t="e">
         <f>(H4/1000)/(MAX($C$4:$E$14)-MIN($C$4:$E$14))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K4">
-        <f>J4*14.5038</f>
+      <c r="K4" s="37">
         <v>0</v>
       </c>
-      <c r="L4">
-        <f>J4*100</f>
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <f>K4*6.89476</f>
-        <v>0</v>
+      <c r="L4" s="38"/>
+      <c r="M4" s="39"/>
+      <c r="O4" t="s">
+        <v>24</v>
+      </c>
+      <c r="T4" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B5" s="8">
+        <v>25</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="10">
         <f>(C5+D5+E5)/3</f>
         <v>0</v>
       </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="8">
-        <f t="shared" ref="H5:H14" si="0">MAX(C5-F5,D5-F5,E5-F5)*1000</f>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10">
+        <f t="shared" ref="H5:H17" si="0">MAX(C5-F5,D5-F5,E5-F5)*1000</f>
         <v>0</v>
       </c>
-      <c r="I5" s="12" t="e">
-        <f t="shared" ref="I5:I14" si="1">(H5/1000)/(MAX($C$4:$E$14)-MIN($C$4:$E$14))</f>
+      <c r="I5" s="11" t="e">
+        <f t="shared" ref="I5:I17" si="1">(H5/1000)/(MAX($C$4:$E$14)-MIN($C$4:$E$14))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J5">
-        <v>0.05</v>
-      </c>
-      <c r="K5">
-        <f>J5*14.5038</f>
-        <v>0.72519</v>
-      </c>
-      <c r="L5">
-        <f>J5*100</f>
-        <v>5</v>
-      </c>
-      <c r="M5">
-        <f>K5*6.89476</f>
-        <v>5.0000110044000001</v>
+      <c r="K5" s="5">
+        <v>25</v>
+      </c>
+      <c r="L5" s="3"/>
+      <c r="M5" s="35"/>
+      <c r="O5" t="s">
+        <v>30</v>
+      </c>
+      <c r="T5" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="U5" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="V5" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="W5" s="26" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="9">
-        <v>1</v>
-      </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11">
-        <f t="shared" ref="F6:F14" si="2">(C6+D6+E6)/3</f>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B6" s="8">
+        <v>50</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="10">
+        <f t="shared" ref="F6:F17" si="2">(C6+D6+E6)/3</f>
         <v>0</v>
       </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="8">
+      <c r="G6" s="10"/>
+      <c r="H6" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I6" s="12" t="e">
+      <c r="I6" s="11" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J6">
-        <v>0.1</v>
-      </c>
-      <c r="K6">
-        <f t="shared" ref="K6:K14" si="3">J6*14.5038</f>
-        <v>1.45038</v>
-      </c>
-      <c r="L6">
-        <f t="shared" ref="L6:L14" si="4">J6*100</f>
-        <v>10</v>
-      </c>
-      <c r="M6">
-        <f t="shared" ref="M6:M14" si="5">K6*6.89476</f>
-        <v>10.0000220088</v>
+      <c r="K6" s="5">
+        <v>50</v>
+      </c>
+      <c r="L6" s="3"/>
+      <c r="M6" s="35"/>
+      <c r="U6">
+        <f>T6*14.5038</f>
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <f>T6*100</f>
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <f>U6*6.89476</f>
+        <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="9">
-        <v>1.5</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B7" s="8">
+        <v>75</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="8">
+      <c r="G7" s="10"/>
+      <c r="H7" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I7" s="12" t="e">
+      <c r="I7" s="11" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J7">
+      <c r="K7" s="5">
+        <v>75</v>
+      </c>
+      <c r="L7" s="3"/>
+      <c r="M7" s="35"/>
+      <c r="T7">
+        <v>0.05</v>
+      </c>
+      <c r="U7">
+        <f>T7*14.5038</f>
+        <v>0.72519</v>
+      </c>
+      <c r="V7">
+        <f>T7*100</f>
+        <v>5</v>
+      </c>
+      <c r="W7">
+        <f>U7*6.89476</f>
+        <v>5.0000110044000001</v>
+      </c>
+    </row>
+    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B8" s="8">
+        <v>100</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="11" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K8" s="5">
+        <v>100</v>
+      </c>
+      <c r="L8" s="3"/>
+      <c r="M8" s="35"/>
+      <c r="T8">
+        <v>0.1</v>
+      </c>
+      <c r="U8">
+        <f t="shared" ref="U8:U16" si="3">T8*14.5038</f>
+        <v>1.45038</v>
+      </c>
+      <c r="V8">
+        <f t="shared" ref="V8:V16" si="4">T8*100</f>
+        <v>10</v>
+      </c>
+      <c r="W8">
+        <f t="shared" ref="W8:W16" si="5">U8*6.89476</f>
+        <v>10.0000220088</v>
+      </c>
+    </row>
+    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B9" s="8">
+        <v>125</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="11" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K9" s="5">
+        <v>125</v>
+      </c>
+      <c r="L9" s="3"/>
+      <c r="M9" s="35"/>
+      <c r="T9">
         <v>0.15</v>
       </c>
-      <c r="K7">
+      <c r="U9">
         <f t="shared" si="3"/>
         <v>2.17557</v>
       </c>
-      <c r="L7">
+      <c r="V9">
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="M7">
+      <c r="W9">
         <f t="shared" si="5"/>
         <v>15.000033013199999</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="9">
-        <v>2</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="11">
+    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B10" s="8">
+        <v>150</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="8">
+      <c r="G10" s="10"/>
+      <c r="H10" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I8" s="12" t="e">
+      <c r="I10" s="11" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J8">
+      <c r="K10" s="5">
+        <v>150</v>
+      </c>
+      <c r="L10" s="3"/>
+      <c r="M10" s="35"/>
+      <c r="T10">
         <v>0.2</v>
       </c>
-      <c r="K8">
+      <c r="U10">
         <f t="shared" si="3"/>
         <v>2.90076</v>
       </c>
-      <c r="L8">
+      <c r="V10">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
-      <c r="M8">
+      <c r="W10">
         <f t="shared" si="5"/>
         <v>20.000044017600001</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="11">
+    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B11" s="8">
+        <v>175</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="8">
+      <c r="G11" s="10"/>
+      <c r="H11" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I9" s="12" t="e">
+      <c r="I11" s="11" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J9">
+      <c r="K11" s="5">
+        <v>175</v>
+      </c>
+      <c r="L11" s="3"/>
+      <c r="M11" s="35"/>
+      <c r="T11">
         <v>0.25</v>
       </c>
-      <c r="K9">
+      <c r="U11">
         <f t="shared" si="3"/>
         <v>3.62595</v>
       </c>
-      <c r="L9">
+      <c r="V11">
         <f t="shared" si="4"/>
         <v>25</v>
       </c>
-      <c r="M9">
+      <c r="W11">
         <f t="shared" si="5"/>
         <v>25.000055021999998</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="11">
+    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B12" s="8">
+        <v>200</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G10" s="11"/>
-      <c r="H10" s="8">
+      <c r="G12" s="10"/>
+      <c r="H12" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I10" s="12" t="e">
+      <c r="I12" s="11" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J10">
+      <c r="K12" s="5">
+        <v>200</v>
+      </c>
+      <c r="L12" s="3"/>
+      <c r="M12" s="35"/>
+      <c r="T12">
         <v>0.3</v>
       </c>
-      <c r="K10">
+      <c r="U12">
         <f t="shared" si="3"/>
         <v>4.35114</v>
       </c>
-      <c r="L10">
+      <c r="V12">
         <f t="shared" si="4"/>
         <v>30</v>
       </c>
-      <c r="M10">
+      <c r="W12">
         <f t="shared" si="5"/>
         <v>30.000066026399999</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="11">
+    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B13" s="8">
+        <v>225</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="8">
+      <c r="G13" s="10"/>
+      <c r="H13" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I11" s="12" t="e">
+      <c r="I13" s="11" t="e">
+        <f>(H13/1000)/(MAX($C$4:$E$14)-MIN($C$4:$E$14))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K13" s="5">
+        <v>225</v>
+      </c>
+      <c r="L13" s="3"/>
+      <c r="M13" s="35"/>
+      <c r="T13">
+        <v>0.35</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="3"/>
+        <v>5.0763299999999996</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="4"/>
+        <v>35</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="5"/>
+        <v>35.000077030799993</v>
+      </c>
+    </row>
+    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B14" s="8">
+        <v>250</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="11" t="e">
+        <f>(H14/1000)/(MAX($C$4:$E$14)-MIN($C$4:$E$14))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K14" s="5">
+        <v>250</v>
+      </c>
+      <c r="L14" s="3"/>
+      <c r="M14" s="35"/>
+      <c r="T14">
+        <v>0.4</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="3"/>
+        <v>5.80152</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="5"/>
+        <v>40.000088035200001</v>
+      </c>
+    </row>
+    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B15" s="8">
+        <v>275</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="11" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J11">
-        <v>0.35</v>
-      </c>
-      <c r="K11">
+      <c r="K15" s="5">
+        <v>275</v>
+      </c>
+      <c r="L15" s="3"/>
+      <c r="M15" s="35"/>
+      <c r="T15">
+        <v>0.45</v>
+      </c>
+      <c r="U15">
         <f t="shared" si="3"/>
-        <v>5.0763299999999996</v>
-      </c>
-      <c r="L11">
+        <v>6.5267100000000005</v>
+      </c>
+      <c r="V15">
         <f t="shared" si="4"/>
-        <v>35</v>
-      </c>
-      <c r="M11">
+        <v>45</v>
+      </c>
+      <c r="W15">
         <f t="shared" si="5"/>
-        <v>35.000077030799993</v>
+        <v>45.000099039600002</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="11">
+    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B16" s="32">
+        <v>280</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="8">
+      <c r="G16" s="4"/>
+      <c r="H16" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I12" s="12" t="e">
+      <c r="I16" s="11" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J12">
-        <v>0.4</v>
-      </c>
-      <c r="K12">
+      <c r="K16" s="32">
+        <v>280</v>
+      </c>
+      <c r="L16" s="3"/>
+      <c r="M16" s="35"/>
+      <c r="T16">
+        <v>0.5</v>
+      </c>
+      <c r="U16">
         <f t="shared" si="3"/>
-        <v>5.80152</v>
-      </c>
-      <c r="L12">
+        <v>7.2519</v>
+      </c>
+      <c r="V16">
         <f t="shared" si="4"/>
-        <v>40</v>
-      </c>
-      <c r="M12">
+        <v>50</v>
+      </c>
+      <c r="W16">
         <f t="shared" si="5"/>
-        <v>40.000088035200001</v>
+        <v>50.000110043999996</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="9"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="11">
+    <row r="17" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="33">
+        <v>295</v>
+      </c>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="13">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="8">
+      <c r="G17" s="13">
+        <f>(F17-F4)/5/1</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I13" s="12" t="e">
+      <c r="I17" s="14" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J13">
-        <v>0.45</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="3"/>
-        <v>6.5267100000000005</v>
-      </c>
-      <c r="L13">
-        <f t="shared" si="4"/>
-        <v>45</v>
-      </c>
-      <c r="M13">
-        <f t="shared" si="5"/>
-        <v>45.000099039600002</v>
-      </c>
+      <c r="K17" s="33">
+        <v>295</v>
+      </c>
+      <c r="L17" s="6"/>
+      <c r="M17" s="36"/>
     </row>
-    <row r="14" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="13"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="15">
-        <f t="shared" si="2"/>
+    <row r="18" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+    </row>
+    <row r="19" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="31"/>
+    </row>
+    <row r="20" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="I20" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B21" s="18">
         <v>0</v>
       </c>
-      <c r="G14" s="15">
-        <f>(F14-F4)/5/1</f>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="20">
+        <f>(C21+D21+E21)/3</f>
         <v>0</v>
       </c>
-      <c r="H14" s="24">
-        <f t="shared" si="0"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20">
+        <f>MAX(C21-F21,D21-F21,E21-F21)*1000</f>
         <v>0</v>
       </c>
-      <c r="I14" s="16" t="e">
-        <f t="shared" si="1"/>
+      <c r="I21" s="21" t="e">
+        <f>(H21/1000)/(MAX($C$4:$E$14)-MIN($C$4:$E$14))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J14">
-        <v>0.5</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="3"/>
-        <v>7.2519</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="4"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22" s="8">
+        <v>25</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="10">
+        <f>(C22+D22+E22)/3</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10">
+        <f t="shared" ref="H22:H34" si="6">MAX(C22-F22,D22-F22,E22-F22)*1000</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="11" t="e">
+        <f t="shared" ref="I22:I34" si="7">(H22/1000)/(MAX($C$4:$E$14)-MIN($C$4:$E$14))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B23" s="8">
         <v>50</v>
       </c>
-      <c r="M14">
-        <f t="shared" si="5"/>
-        <v>50.000110043999996</v>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="10">
+        <f t="shared" ref="F23:F34" si="8">(C23+D23+E23)/3</f>
+        <v>0</v>
+      </c>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="11" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B24" s="8">
+        <v>75</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="10">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="11" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="37"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="35"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="37"/>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="35"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="37"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="35"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="37"/>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="37"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="35"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="37"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="35"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="37"/>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B25" s="8">
+        <v>100</v>
+      </c>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="10">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="11" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="35"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="37"/>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B26" s="8">
+        <v>125</v>
+      </c>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="10">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="11" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="37"/>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B27" s="8">
+        <v>150</v>
+      </c>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="10">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I27" s="11" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="35"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="37"/>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B28" s="8">
+        <v>175</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="10">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="11" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="37"/>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B29" s="8">
+        <v>200</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="10">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I29" s="11" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B30" s="8">
+        <v>225</v>
+      </c>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="10">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I30" s="11" t="e">
+        <f>(H30/1000)/(MAX($C$4:$E$14)-MIN($C$4:$E$14))</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B31" s="8">
+        <v>250</v>
+      </c>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="10">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G31" s="4"/>
+      <c r="H31" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I31" s="11" t="e">
+        <f>(H31/1000)/(MAX($C$4:$E$14)-MIN($C$4:$E$14))</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="8">
+        <v>275</v>
+      </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="10">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G32" s="4"/>
+      <c r="H32" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I32" s="11" t="e">
+        <f t="shared" ref="I32:I34" si="9">(H32/1000)/(MAX($C$4:$E$14)-MIN($C$4:$E$14))</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B33" s="32">
+        <v>280</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="10">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G33" s="4"/>
+      <c r="H33" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I33" s="11" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="33">
+        <v>295</v>
+      </c>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="13">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G34" s="13">
+        <f>(F34-F21)/5/1</f>
+        <v>0</v>
+      </c>
+      <c r="H34" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I34" s="14" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="L34" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B17:I17"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="K2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8868,8 +9580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91D8B8CD-DCC6-4C90-A9E8-3306C55A5ABE}">
   <dimension ref="B1:H29"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8895,56 +9607,56 @@
       <c r="H2" s="31"/>
     </row>
     <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="28" t="s">
+      <c r="H3" s="25" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="20">
+      <c r="B4" s="18">
         <v>0</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="16">
         <v>0.13159999999999999</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="16">
         <v>0.1424</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="16">
         <v>0.1507</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="17">
         <f>(C4+D4+E4)/3</f>
         <v>0.14156666666666667</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G4" s="20">
         <f t="shared" ref="G4:G14" si="0">MAX(C4-F4,D4-F4,E4-F4)*1000</f>
         <v>9.1333333333333258</v>
       </c>
-      <c r="H4" s="23">
+      <c r="H4" s="21">
         <f>(G4/1000)/(MAX($C$4:$E$14)-MIN($C$4:$E$14))</f>
         <v>2.365780794004384E-3</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>0.25</v>
       </c>
       <c r="C5" s="3">
@@ -8960,17 +9672,17 @@
         <f t="shared" ref="F5:F14" si="1">(C5+D5+E5)/3</f>
         <v>0.40420000000000006</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="10">
         <f t="shared" si="0"/>
         <v>9.9999999999933475E-2</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="11">
         <f>(G5/1000)/(MAX($C$4:$E$14)-MIN($C$4:$E$14))</f>
         <v>2.5902709423388456E-5</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>0.5</v>
       </c>
       <c r="C6" s="3">
@@ -8986,17 +9698,17 @@
         <f t="shared" si="1"/>
         <v>0.80723333333333336</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="10">
         <f t="shared" si="0"/>
         <v>0.96666666666667123</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="11">
         <f t="shared" ref="H6:H14" si="2">(G6/1000)/(MAX($C$4:$E$14)-MIN($C$4:$E$14))</f>
         <v>2.5039285775958954E-4</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>0.75</v>
       </c>
       <c r="C7" s="3">
@@ -9012,17 +9724,17 @@
         <f t="shared" si="1"/>
         <v>1.2085999999999999</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="10">
         <f t="shared" si="0"/>
         <v>0.300000000000189</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="11">
         <f t="shared" si="2"/>
         <v>7.7708128270266027E-5</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="9">
+      <c r="B8" s="8">
         <v>1</v>
       </c>
       <c r="C8" s="3">
@@ -9038,17 +9750,17 @@
         <f t="shared" si="1"/>
         <v>1.6104666666666667</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="10">
         <f t="shared" si="0"/>
         <v>0.23333333333330764</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="11">
         <f t="shared" si="2"/>
         <v>6.0439655321273288E-5</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>1.25</v>
       </c>
       <c r="C9" s="3">
@@ -9064,17 +9776,17 @@
         <f t="shared" si="1"/>
         <v>2.0110333333333337</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="10">
         <f t="shared" si="0"/>
         <v>0.26666666666619321</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="11">
         <f t="shared" si="2"/>
         <v>6.9073891795625865E-5</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="9">
+      <c r="B10" s="8">
         <v>1.5</v>
       </c>
       <c r="C10" s="3">
@@ -9090,17 +9802,17 @@
         <f t="shared" si="1"/>
         <v>2.4111666666666665</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="10">
         <f t="shared" si="0"/>
         <v>0.63333333333348563</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="11">
         <f t="shared" si="2"/>
         <v>1.6405049301494216E-4</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="9">
+      <c r="B11" s="8">
         <v>1.75</v>
       </c>
       <c r="C11" s="3">
@@ -9116,17 +9828,17 @@
         <f t="shared" si="1"/>
         <v>2.8097333333333334</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="10">
         <f t="shared" si="0"/>
         <v>0.16666666666642627</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="11">
         <f t="shared" si="2"/>
         <v>4.3171182372280543E-5</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="9">
+      <c r="B12" s="8">
         <v>2</v>
       </c>
       <c r="C12" s="3">
@@ -9142,17 +9854,17 @@
         <f t="shared" si="1"/>
         <v>3.2057333333333333</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="10">
         <f t="shared" si="0"/>
         <v>0.46666666666661527</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="11">
         <f t="shared" si="2"/>
         <v>1.2087931064254658E-4</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="9">
+      <c r="B13" s="8">
         <v>2.25</v>
       </c>
       <c r="C13" s="3">
@@ -9168,17 +9880,17 @@
         <f t="shared" si="1"/>
         <v>3.6005666666666669</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="10">
         <f t="shared" si="0"/>
         <v>2.7333333333330323</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="11">
         <f t="shared" si="2"/>
         <v>7.0800739090634416E-4</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="13">
+      <c r="B14" s="12">
         <v>2.5</v>
       </c>
       <c r="C14" s="6">
@@ -9194,11 +9906,11 @@
         <f t="shared" si="1"/>
         <v>3.9918333333333336</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G14" s="13">
         <f t="shared" si="0"/>
         <v>0.36666666666640424</v>
       </c>
-      <c r="H14" s="16">
+      <c r="H14" s="14">
         <f t="shared" si="2"/>
         <v>9.4976601219086214E-5</v>
       </c>
@@ -9221,50 +9933,50 @@
       <c r="H17" s="31"/>
     </row>
     <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="27" t="s">
+      <c r="D18" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="27" t="s">
+      <c r="E18" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="25" t="s">
+      <c r="F18" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="27" t="s">
+      <c r="G18" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="H18" s="28" t="s">
+      <c r="H18" s="25" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="17">
+      <c r="B19" s="15">
         <v>0</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="16">
         <v>0.14149999999999999</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="16">
         <v>0.1368</v>
       </c>
-      <c r="E19" s="18">
+      <c r="E19" s="16">
         <v>0.1356</v>
       </c>
-      <c r="F19" s="19">
+      <c r="F19" s="17">
         <f t="shared" ref="F19:F29" si="3">(C19+D19+E19)/3</f>
         <v>0.13796666666666665</v>
       </c>
-      <c r="G19" s="19">
+      <c r="G19" s="17">
         <f t="shared" ref="G19:G29" si="4">MAX(C19-F19,D19-F19,E19-F19)*1000</f>
         <v>3.5333333333333328</v>
       </c>
-      <c r="H19" s="23">
+      <c r="H19" s="21">
         <f>(G19/1000)/(MAX($C$19:$E$29)-MIN($C$19:$E$29))</f>
         <v>9.1617832633234789E-4</v>
       </c>
@@ -9290,7 +10002,7 @@
         <f t="shared" si="4"/>
         <v>9.9999999999988987E-2</v>
       </c>
-      <c r="H20" s="12">
+      <c r="H20" s="11">
         <f t="shared" ref="H20:H28" si="5">(G20/1000)/(MAX($C$19:$E$29)-MIN($C$19:$E$29))</f>
         <v>2.5929575273554164E-5</v>
       </c>
@@ -9316,7 +10028,7 @@
         <f t="shared" si="4"/>
         <v>9.9999999999988987E-2</v>
       </c>
-      <c r="H21" s="12">
+      <c r="H21" s="11">
         <f t="shared" si="5"/>
         <v>2.5929575273554164E-5</v>
       </c>
@@ -9342,7 +10054,7 @@
         <f t="shared" si="4"/>
         <v>9.9999999999988987E-2</v>
       </c>
-      <c r="H22" s="12">
+      <c r="H22" s="11">
         <f t="shared" si="5"/>
         <v>2.5929575273554164E-5</v>
       </c>
@@ -9368,7 +10080,7 @@
         <f t="shared" si="4"/>
         <v>9.9999999999766942E-2</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H23" s="11">
         <f t="shared" si="5"/>
         <v>2.5929575273496589E-5</v>
       </c>
@@ -9394,7 +10106,7 @@
         <f t="shared" si="4"/>
         <v>9.9999999999766942E-2</v>
       </c>
-      <c r="H24" s="12">
+      <c r="H24" s="11">
         <f t="shared" si="5"/>
         <v>2.5929575273496589E-5</v>
       </c>
@@ -9420,7 +10132,7 @@
         <f t="shared" si="4"/>
         <v>0.19999999999997797</v>
       </c>
-      <c r="H25" s="12">
+      <c r="H25" s="11">
         <f t="shared" si="5"/>
         <v>5.1859150547108328E-5</v>
       </c>
@@ -9446,7 +10158,7 @@
         <f t="shared" si="4"/>
         <v>0.16666666666687036</v>
       </c>
-      <c r="H26" s="12">
+      <c r="H26" s="11">
         <f t="shared" si="5"/>
         <v>4.3215958789314516E-5</v>
       </c>
@@ -9472,7 +10184,7 @@
         <f t="shared" si="4"/>
         <v>0.46666666666661527</v>
       </c>
-      <c r="H27" s="12">
+      <c r="H27" s="11">
         <f t="shared" si="5"/>
         <v>1.2100468460991944E-4</v>
       </c>
@@ -9498,13 +10210,13 @@
         <f t="shared" si="4"/>
         <v>0.43333333333350765</v>
       </c>
-      <c r="H28" s="12">
+      <c r="H28" s="11">
         <f t="shared" si="5"/>
         <v>1.1236149285212562E-4</v>
       </c>
     </row>
     <row r="29" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="13">
+      <c r="B29" s="12">
         <v>2.5</v>
       </c>
       <c r="C29" s="6">
@@ -9520,11 +10232,11 @@
         <f t="shared" si="3"/>
         <v>3.9918333333333336</v>
       </c>
-      <c r="G29" s="15">
+      <c r="G29" s="13">
         <f t="shared" si="4"/>
         <v>0.36666666666640424</v>
       </c>
-      <c r="H29" s="16">
+      <c r="H29" s="14">
         <f>(G29/1000)/(MAX($C$19:$E$29)-MIN($C$19:$E$29))</f>
         <v>9.5075109336307701E-5</v>
       </c>

</xml_diff>